<commit_message>
ad RandomForrest to boxplot
</commit_message>
<xml_diff>
--- a/results/Comparison_preprocessing_weka.xlsx
+++ b/results/Comparison_preprocessing_weka.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Dataset</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t xml:space="preserve">Avg time to build model: </t>
+  </si>
+  <si>
+    <t>Random Forrest</t>
   </si>
 </sst>
 </file>
@@ -408,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -420,10 +423,10 @@
     <col min="3" max="3" width="24" customWidth="1"/>
     <col min="4" max="4" width="19" customWidth="1"/>
     <col min="5" max="5" width="21" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -439,8 +442,11 @@
       <c r="F1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -456,8 +462,11 @@
       <c r="F2">
         <v>0.64500000000000002</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2">
+        <v>0.81599999999999995</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -473,8 +482,11 @@
       <c r="F3">
         <v>0.64300000000000002</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <v>0.81599999999999995</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -490,8 +502,11 @@
       <c r="F4">
         <v>0.63500000000000001</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <v>0.82099999999999995</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -507,8 +522,11 @@
       <c r="F5">
         <v>0.65400000000000003</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5">
+        <v>0.81100000000000005</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -524,8 +542,11 @@
       <c r="F6">
         <v>0.64700000000000002</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <v>0.82499999999999996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -541,8 +562,11 @@
       <c r="F7">
         <v>0.63700000000000001</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7">
+        <v>0.82399999999999995</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -558,8 +582,11 @@
       <c r="F8">
         <v>0.63700000000000001</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8">
+        <v>0.82599999999999996</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -575,8 +602,11 @@
       <c r="F9">
         <v>0.64200000000000002</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9">
+        <v>0.81699999999999995</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -592,8 +622,11 @@
       <c r="F10">
         <v>0.63200000000000001</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10">
+        <v>0.82399999999999995</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -609,8 +642,11 @@
       <c r="F11">
         <v>0.64700000000000002</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11">
+        <v>0.82899999999999996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -626,8 +662,11 @@
       <c r="F12">
         <v>0.63900000000000001</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12">
+        <v>0.82099999999999995</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -643,8 +682,11 @@
       <c r="F13">
         <v>0.63800000000000001</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13">
+        <v>0.82399999999999995</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -660,10 +702,13 @@
       <c r="F17">
         <v>1.21</v>
       </c>
+      <c r="G17">
+        <v>16.850000000000001</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C13">
-    <cfRule type="colorScale" priority="12">
+    <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -673,7 +718,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E20">
-    <cfRule type="colorScale" priority="9">
+    <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -683,7 +728,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D13">
-    <cfRule type="colorScale" priority="7">
+    <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -693,6 +738,16 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E13">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F13 G2">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -702,7 +757,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F13">
+  <conditionalFormatting sqref="C2:F15 G2">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -712,18 +767,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:F15">
+  <conditionalFormatting sqref="C2:F13 G2">
     <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C2:F13">
-    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -733,7 +778,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="1">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -743,7 +788,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="colorScale" priority="2">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2:G13">
+    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>

</xml_diff>